<commit_message>
modificaciones footer ,index ,registrate ,crea tu tienda
</commit_message>
<xml_diff>
--- a/excel/maquetacionint (1).xlsx
+++ b/excel/maquetacionint (1).xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyectos HTML\city shop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Registro Usuario" sheetId="2" r:id="rId1"/>
-    <sheet name="Login" sheetId="5" r:id="rId2"/>
-    <sheet name="sss" sheetId="1" r:id="rId3"/>
-    <sheet name="Interfaz" sheetId="4" r:id="rId4"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId5"/>
+    <sheet name="Login" sheetId="5" r:id="rId1"/>
+    <sheet name="Registro Usuario" sheetId="2" r:id="rId2"/>
+    <sheet name="Interfaz" sheetId="4" r:id="rId3"/>
+    <sheet name="sss" sheetId="1" r:id="rId4"/>
+    <sheet name="administracion Tienda" sheetId="6" r:id="rId5"/>
+    <sheet name="proyecto ingreso datos" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>nombre tienda</t>
   </si>
@@ -235,6 +236,18 @@
   </si>
   <si>
     <t>Correo electronico</t>
+  </si>
+  <si>
+    <t>Interfaz Usuario</t>
+  </si>
+  <si>
+    <t>ech123</t>
+  </si>
+  <si>
+    <t>Vea Su local</t>
+  </si>
+  <si>
+    <t>Modificación productos</t>
   </si>
 </sst>
 </file>
@@ -242,9 +255,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +284,13 @@
     <font>
       <b/>
       <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -667,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -705,16 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -723,9 +734,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -745,30 +753,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -776,42 +763,111 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -820,53 +876,39 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,6 +1234,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="54"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="49">
+        <v>10338484</v>
+      </c>
+      <c r="F4" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+    </row>
+    <row r="5" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F6" s="89" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="88"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F6:J9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1207,520 +1332,520 @@
   <sheetData>
     <row r="2" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="54"/>
-      <c r="D3" s="92" t="s">
+      <c r="C3" s="43"/>
+      <c r="D3" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="61"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="49"/>
     </row>
     <row r="4" spans="3:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="55"/>
-      <c r="D4" s="62" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="58"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="47"/>
     </row>
     <row r="5" spans="3:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C5" s="55"/>
-      <c r="D5" s="34" t="s">
+      <c r="C5" s="44"/>
+      <c r="D5" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="78" t="s">
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="58"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="47"/>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="55"/>
-      <c r="D6" s="34" t="s">
+      <c r="C6" s="44"/>
+      <c r="D6" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="63"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="58"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="47"/>
     </row>
     <row r="7" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="55"/>
-      <c r="D7" s="36" t="s">
+      <c r="C7" s="44"/>
+      <c r="D7" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="58"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="47"/>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="55"/>
-      <c r="D8" s="34" t="s">
+      <c r="C8" s="44"/>
+      <c r="D8" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="58"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="47"/>
     </row>
     <row r="9" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="55"/>
-      <c r="D9" s="34" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="58"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="47"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="55"/>
-      <c r="D10" s="34" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="91"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="58"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="47"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="55"/>
-      <c r="D11" s="36" t="s">
+      <c r="C11" s="44"/>
+      <c r="D11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="91"/>
-      <c r="I11" s="91"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="58"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="47"/>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="55"/>
-      <c r="D12" s="36" t="s">
+      <c r="C12" s="44"/>
+      <c r="D12" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="91"/>
-      <c r="I12" s="91"/>
-      <c r="J12" s="91"/>
-      <c r="K12" s="58"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="47"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="55"/>
-      <c r="D13" s="36" t="s">
+      <c r="C13" s="44"/>
+      <c r="D13" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="58"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="47"/>
     </row>
     <row r="14" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="55"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
     </row>
     <row r="15" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="55"/>
-      <c r="D15" s="49" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="86" t="s">
+      <c r="F15" s="46"/>
+      <c r="G15" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="58"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="47"/>
     </row>
     <row r="16" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="55"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="88" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="89"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="58"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="55"/>
-      <c r="D17" s="47" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="58"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="55"/>
-      <c r="D18" s="41" t="s">
+      <c r="C18" s="44"/>
+      <c r="D18" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="58"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="47"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="55"/>
-      <c r="D19" s="43" t="s">
+      <c r="C19" s="44"/>
+      <c r="D19" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="58"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="47"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="55"/>
-      <c r="D20" s="43" t="s">
+      <c r="C20" s="44"/>
+      <c r="D20" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="58"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="55"/>
-      <c r="D21" s="43" t="s">
+      <c r="C21" s="44"/>
+      <c r="D21" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="58"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="47"/>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="55"/>
-      <c r="D22" s="43" t="s">
+      <c r="C22" s="44"/>
+      <c r="D22" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="58"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="47"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="55"/>
-      <c r="D23" s="43" t="s">
+      <c r="C23" s="44"/>
+      <c r="D23" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="58"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="47"/>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="55"/>
-      <c r="D24" s="43" t="s">
+      <c r="C24" s="44"/>
+      <c r="D24" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="58"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="47"/>
     </row>
     <row r="25" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="55"/>
-      <c r="D25" s="44" t="s">
+      <c r="C25" s="44"/>
+      <c r="D25" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="58"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="47"/>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="55"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="58"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="47"/>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="55"/>
-      <c r="D27" s="45" t="s">
+      <c r="C27" s="44"/>
+      <c r="D27" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="58"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="47"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="55"/>
-      <c r="D28" s="35" t="s">
+      <c r="C28" s="44"/>
+      <c r="D28" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="58"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="47"/>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="55"/>
-      <c r="D29" s="35" t="s">
+      <c r="C29" s="44"/>
+      <c r="D29" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="58"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="47"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="55"/>
-      <c r="D30" s="35" t="s">
+      <c r="C30" s="44"/>
+      <c r="D30" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="58"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="47"/>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="55"/>
-      <c r="D31" s="35" t="s">
+      <c r="C31" s="44"/>
+      <c r="D31" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="58"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="47"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="55"/>
-      <c r="D32" s="35" t="s">
+      <c r="C32" s="44"/>
+      <c r="D32" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="58"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="47"/>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C33" s="55"/>
-      <c r="D33" s="35" t="s">
+      <c r="C33" s="44"/>
+      <c r="D33" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="58"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="47"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="55"/>
-      <c r="D34" s="46" t="s">
+      <c r="C34" s="44"/>
+      <c r="D34" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="58"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="47"/>
     </row>
     <row r="35" spans="3:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C35" s="55"/>
-      <c r="D35" s="93" t="s">
+      <c r="C35" s="44"/>
+      <c r="D35" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="57"/>
-      <c r="K35" s="58"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="47"/>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="55"/>
-      <c r="D36" s="35" t="s">
+      <c r="C36" s="44"/>
+      <c r="D36" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="58"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="47"/>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C37" s="55"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="58"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="47"/>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="55"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="58"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="47"/>
     </row>
     <row r="39" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="55"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="57"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="57"/>
-      <c r="K39" s="58"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="47"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="55"/>
-      <c r="D40" s="50" t="s">
+      <c r="C40" s="44"/>
+      <c r="D40" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="51"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="67" t="s">
+      <c r="E40" s="63"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="68"/>
-      <c r="I40" s="68"/>
-      <c r="J40" s="69"/>
-      <c r="K40" s="58"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="68"/>
+      <c r="K40" s="47"/>
     </row>
     <row r="41" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="55"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="72"/>
-      <c r="K41" s="58"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="47"/>
     </row>
     <row r="42" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="56"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="66"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1743,90 +1868,156 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J9"/>
+  <dimension ref="C4:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="73"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="61">
-        <v>10338484</v>
-      </c>
-      <c r="F4" s="76" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-    </row>
-    <row r="5" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="66" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F6" s="77" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="76"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="73" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="93" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="93"/>
+    </row>
+    <row r="5" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="90"/>
+      <c r="D10" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="91"/>
+      <c r="D11" s="29"/>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="91"/>
+      <c r="D12" s="23">
+        <v>65500</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="91"/>
+      <c r="D13" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="92"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="10">
+        <v>65656565</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F6:J9"/>
+  <mergeCells count="2">
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -1856,22 +2047,22 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="27" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="11"/>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="28" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1971,161 +2162,96 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:D28"/>
+  <dimension ref="C2:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="33"/>
-    </row>
-    <row r="5" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="23"/>
-      <c r="D10" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="24"/>
-      <c r="D11" s="32"/>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="24"/>
-      <c r="D12" s="26">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="24"/>
-      <c r="D13" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="25"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="10">
-        <v>65656565</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="6"/>
+    <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="95" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="5"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="96" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="98"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C4:D4"/>
+  <mergeCells count="3">
+    <mergeCell ref="F5:J6"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="C5:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>